<commit_message>
removed gimbal/camera payloads from messages
</commit_message>
<xml_diff>
--- a/TA2/lmcp-message-format/LMCP messages.xlsx
+++ b/TA2/lmcp-message-format/LMCP messages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21105" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21105" windowHeight="3600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="268">
   <si>
     <t>$</t>
   </si>
@@ -464,45 +464,15 @@
     <t>Air Vehicle State</t>
   </si>
   <si>
-    <t>Entity state</t>
-  </si>
-  <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <t>Centerpoint</t>
-  </si>
-  <si>
     <t>Location3D</t>
   </si>
   <si>
-    <t>Gimbal State</t>
-  </si>
-  <si>
-    <t>Payload State</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Camera State</t>
-  </si>
-  <si>
-    <t>Gimballed Payload State</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
     <t>AirVehicleState</t>
   </si>
   <si>
-    <t>Entity ID</t>
-  </si>
-  <si>
-    <t>x-direction velocity</t>
-  </si>
-  <si>
     <t>y-direction velocity</t>
   </si>
   <si>
@@ -551,12 +521,6 @@
     <t>Payload state list size</t>
   </si>
   <si>
-    <t>Payload ID (8 bytes)</t>
-  </si>
-  <si>
-    <t>Num parameters</t>
-  </si>
-  <si>
     <t>Key Length (2 bytes)</t>
   </si>
   <si>
@@ -569,27 +533,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Pointing Mode</t>
-  </si>
-  <si>
-    <t>Azimuth</t>
-  </si>
-  <si>
-    <t>Elevation</t>
-  </si>
-  <si>
-    <t>Rotation</t>
-  </si>
-  <si>
-    <t>Horizontal field of view</t>
-  </si>
-  <si>
-    <t>Vertical field of view</t>
-  </si>
-  <si>
-    <t>Footprint size</t>
-  </si>
-  <si>
     <t>Current Waypoint</t>
   </si>
   <si>
@@ -701,60 +644,9 @@
     <t xml:space="preserve">00 02 </t>
   </si>
   <si>
-    <t xml:space="preserve">00 00 00 1B </t>
-  </si>
-  <si>
     <t xml:space="preserve">00 00 00 00 00 00 00 01 </t>
   </si>
   <si>
-    <t>C2 70 00 00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00 00 00 15 </t>
-  </si>
-  <si>
-    <t>00 00 00 00 00 00 27 11</t>
-  </si>
-  <si>
-    <t>42 34 00 00</t>
-  </si>
-  <si>
-    <t>42 07 00 00</t>
-  </si>
-  <si>
-    <t>00 04</t>
-  </si>
-  <si>
-    <t>40 46 A8 4A CA B8 59 E5</t>
-  </si>
-  <si>
-    <t>C0 5E 3E 5C 82 F5 CD 81</t>
-  </si>
-  <si>
-    <t>40 46 A7 DE E2 2E 07 46</t>
-  </si>
-  <si>
-    <t>C0 5E 3F 24 B4 A1 86 CD</t>
-  </si>
-  <si>
-    <t>40 46 A8 62 2A 06 D4 4E</t>
-  </si>
-  <si>
-    <t>C0 5E 3F 5A 99 2C FD 21</t>
-  </si>
-  <si>
-    <t>40 46 A8 D5 F9 47 F4 F9</t>
-  </si>
-  <si>
-    <t>C0 5E 3E EB 32 6B 8C 90</t>
-  </si>
-  <si>
-    <t>40 46 A8 5A 8D C5 49 E7</t>
-  </si>
-  <si>
-    <t>C0 5E 3F 07 EC 63 92 C8</t>
-  </si>
-  <si>
     <t>00 00 00 00 00 00 00 10</t>
   </si>
   <si>
@@ -773,15 +665,6 @@
     <t>VehicleActionCommand</t>
   </si>
   <si>
-    <t>VehicleAction</t>
-  </si>
-  <si>
-    <t>PayloadAction</t>
-  </si>
-  <si>
-    <t>GimbalAngleAction</t>
-  </si>
-  <si>
     <t>Waypoint</t>
   </si>
   <si>
@@ -800,21 +683,6 @@
     <t>Associated tasks length (2 bytes)</t>
   </si>
   <si>
-    <t>Associated task (8 bytes)</t>
-  </si>
-  <si>
-    <t>Payload ID (8 bytes(</t>
-  </si>
-  <si>
-    <t>Asimuth (4 bytes)</t>
-  </si>
-  <si>
-    <t>Elevation (4 bytes)</t>
-  </si>
-  <si>
-    <t>Rotation (4 bytes)</t>
-  </si>
-  <si>
     <t>Status (4 bytes)</t>
   </si>
   <si>
@@ -851,9 +719,6 @@
     <t>Contingency waypoint B (8 bytes)</t>
   </si>
   <si>
-    <t>Associated task (len * 8 bytes)</t>
-  </si>
-  <si>
     <t>Waypoints 2-73</t>
   </si>
   <si>
@@ -881,43 +746,88 @@
     <t xml:space="preserve">24 </t>
   </si>
   <si>
-    <t xml:space="preserve">00 00 1C 44 </t>
-  </si>
-  <si>
     <t xml:space="preserve">00 00 00 33 </t>
   </si>
   <si>
     <t xml:space="preserve">00 00 00 24 </t>
   </si>
   <si>
-    <t xml:space="preserve">00 00 00 17 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2 70 00 00 </t>
-  </si>
-  <si>
     <t xml:space="preserve">00 49 </t>
   </si>
   <si>
     <t xml:space="preserve">00 00 00 23 </t>
   </si>
   <si>
-    <t xml:space="preserve">40 46 A8 82 7F F3 C5 D9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0 5E 3F 68 0B 11 3C B2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">00 00 00 00 00 00 00 02 </t>
   </si>
   <si>
     <t xml:space="preserve">41 B0 00 00 </t>
   </si>
   <si>
-    <t xml:space="preserve">01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 74 A8 2D 02 2A C0 5E 3F 64 A0 29 9B 77 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 02 00 00 00 00 00 00 00 03 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 66 01 AC 0E ED C0 5E 3F 64 F9 5D 68 19 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 03 00 00 00 00 00 00 00 04 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 58 84 9F 07 47 C0 5E 3F 69 0A AE D1 C1 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 04 00 00 00 00 00 00 00 05 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 48 58 B9 CD 4D C0 5E 3F 78 85 08 9B 75 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 05 00 00 00 00 00 00 00 06 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 B5 7E 35 B9 A9 C0 5E 40 D4 79 01 C0 6F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 06 00 00 00 00 00 00 00 07 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 AE CF 8C C6 08 C0 5E 40 DD B9 0A 65 47 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 07 00 00 00 00 00 00 00 08 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 A3 E3 AB 0C 08 C0 5E 40 E4 A7 19 34 7C 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 08 00 00 00 00 00 00 00 09 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 96 2D 89 3C 3A C0 5E 40 E8 53 AB DB 98 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 09 00 00 00 00 00 00 00 0A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 87 85 05 47 10 C0 5E 40 E8 40 51 69 4D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0A 00 00 00 00 00 00 00 0B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 79 E2 92 83 32 C0 5E 40 E4 6F A3 E4 4B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0B 00 00 00 00 00 00 00 0C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6F 1B 69 7A F4 C0 5E 40 DD 64 EE C2 8B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0C 00 00 00 00 00 00 00 0D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 67 3F 52 2D 96 C0 5E 40 CA 80 AF BA EF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0D 00 00 00 00 00 00 00 0E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6E C0 DB 56 DC C0 5E 40 7C 9A F1 E8 B9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0E 00 00 00 00 00 00 00 0F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6B AA FB 77 58 C0 5E 40 75 14 4F A9 E2 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0F 00 00 00 00 00 00 00 10 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 57 83 43 13 C4 C0 5E 40 57 68 54 77 1A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 10 00 00 00 00 00 00 00 11 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 41 B7 7E 6D 5C C0 5E 40 41 3D E2 15 C8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 11 00 00 00 00 00 00 00 12 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 2B 57 F8 B7 8A C0 5E 40 30 C9 94 0F A5 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 12 00 00 00 00 00 00 00 13 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FA E1 35 0E 35 C0 5E 3F EB B8 21 2F 0D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 13 00 00 00 00 00 00 00 14 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF EE 88 C9 28 C0 5E 3F AD A5 7D 31 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 14 00 00 00 00 00 00 00 15 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 1C A7 A6 86 B5 C0 5E 3F 7C 73 19 0E D6 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 15 00 00 00 00 00 00 00 16 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 55 73 6E 47 FE C0 5E 3F 4E 28 29 AB 2A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 16 00 00 00 00 00 00 00 17 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 91 EF 3A 40 7D C0 5E 3F 31 FA D7 F8 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 17 00 00 00 00 00 00 00 18 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 0A 99 E1 B6 E8 C0 5E 3F 14 36 2E 1C B8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 18 00 00 00 00 00 00 00 19 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 1F C8 8A F0 3C C0 5E 3F 0C 14 C9 03 8F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 19 00 00 00 00 00 00 00 1A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 C2 7C 6C D7 38 C0 5E 3E EB E3 1F 4B D0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1A 00 00 00 00 00 00 00 1B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 D5 5D D5 F3 7F C0 5E 3E E5 B9 44 D5 4B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1B 00 00 00 00 00 00 00 1C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 E7 39 3C 77 D7 C0 5E 3E DB 14 37 2E AF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1C 00 00 00 00 00 00 00 1D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 F9 A7 EF 4C B7 C0 5E 3E CB BF 2D B0 35 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1D 00 00 00 00 00 00 00 1E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 09 10 B2 75 AA C0 5E 3E BD 68 C0 50 A4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1E 00 00 00 00 00 00 00 1F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 DF D0 E3 2D 2F C0 5E 3E 89 05 B8 34 27 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1F 00 00 00 00 00 00 00 20 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 D6 DA 71 21 53 C0 5E 3E 6E 8A 52 F5 17 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 20 00 00 00 00 00 00 00 21 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 CD 91 AB 39 64 C0 5E 3E 74 DC BA D8 F5 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 21 00 00 00 00 00 00 00 22 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 9D E1 2D 43 2F C0 5E 3E 7F C4 56 56 2B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 22 00 00 00 00 00 00 00 23 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 7B D8 CB AF 3E C0 5E 3E 7F BE AB 14 4E 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 23 00 00 00 00 00 00 00 24 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 33 39 E2 83 6C C0 5E 3E 8B 7A A6 3B BE 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 24 00 00 00 00 00 00 00 25 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 EC AE 28 6A 9E C0 5E 3E 86 F4 9E 5D 7D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 25 00 00 00 00 00 00 00 26 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 9A 87 32 4D 9C C0 5E 3E 74 A1 DC DB 58 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 26 00 00 00 00 00 00 00 27 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 67 29 AC 98 0F C0 5E 3E 62 CF B9 94 DC 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 27 00 00 00 00 00 00 00 28 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 38 6B 5E 37 F6 C0 5E 3E 46 91 21 7F B8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 28 00 00 00 00 00 00 00 29 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 16 22 81 20 1A C0 5E 3E 1C 2A 08 0C 1F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 29 00 00 00 00 00 00 00 2A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF 6C F8 CD B2 C0 5E 3D E7 76 E6 77 9F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2A 00 00 00 00 00 00 00 2B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF BF E3 EC 87 C0 5E 3D 99 B7 DB 1F 74 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2B 00 00 00 00 00 00 00 2C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 1E B3 03 2D 2F C0 5E 3D 5F 4D 45 67 3F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2C 00 00 00 00 00 00 00 2D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 48 A0 08 48 74 C0 5E 3D 38 89 1A 46 A6 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2D 00 00 00 00 00 00 00 2E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 82 A0 1E 08 A7 C0 5E 3D 11 D1 46 B2 D8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2E 00 00 00 00 00 00 00 2F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 03 0B 1B 06 A3 C0 5E 3C FB F0 4E 6D 13 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2F 00 00 00 00 00 00 00 30 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 21 FA A4 E1 33 C0 5E 3C FC 08 5C 78 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 30 00 00 00 00 00 00 00 31 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 7F C4 EE 6F 65 C0 5E 3C DE 15 82 B9 B4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 31 00 00 00 00 00 00 00 32 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 E1 0C E6 A8 23 C0 5E 3C A2 E2 3C 17 C0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 32 00 00 00 00 00 00 00 33 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 38 92 68 29 D7 C0 5E 3C 78 AC FF 30 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 33 00 00 00 00 00 00 00 34 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 70 13 EB AA 4B C0 5E 3C 62 B0 AB 7B 0A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 34 00 00 00 00 00 00 00 35 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 9D E8 AF B7 5B C0 5E 3C 59 5D 36 68 25 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 35 00 00 00 00 00 00 00 36 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 F6 70 DC 1D 73 C0 5E 3C 56 7B 54 75 F0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 36 00 00 00 00 00 00 00 37 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 83 26 A4 4F 6E C0 5E 3C 66 37 0D C1 1D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 37 00 00 00 00 00 00 00 38 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA AF 49 62 B1 EC C0 5E 3C 86 B9 AB 72 FF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 38 00 00 00 00 00 00 00 39 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA E6 59 92 3E 7C C0 5E 3C F1 D7 6D 0C 3B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 39 00 00 00 00 00 00 00 3A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA EE D4 67 81 69 C0 5E 3C EC B5 A0 DA 28 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3A 00 00 00 00 00 00 00 3B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F7 49 60 7B 1C C0 5E 3C E9 F0 1C 5E C4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3B 00 00 00 00 00 00 00 3C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F7 73 0E 3A AD C0 5E 3C DC 03 C5 D4 2E 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3C 00 00 00 00 00 00 00 3D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F4 BB C9 50 D6 C0 5E 3C CC 46 AF B7 09 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3D 00 00 00 00 00 00 00 3E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA EA 2E 6B C0 CF C0 5E 3C B4 72 53 72 FD 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3E 00 00 00 00 00 00 00 3F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA C1 28 4D 2F 56 C0 5E 3C 93 F3 CD 47 1B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3F 00 00 00 00 00 00 00 40 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 7E 82 25 A6 42 C0 5E 3C 53 8C FF AC B9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 40 00 00 00 00 00 00 00 41 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 18 90 79 49 49 C0 5E 3B FC 3E 1B 37 80 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 41 00 00 00 00 00 00 00 42 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 1D 91 D5 A9 60 C0 5E 3B CD 0F CC E2 9C 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 42 00 00 00 00 00 00 00 43 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 3C 22 AF 05 59 C0 5E 3B 9E A7 F4 65 D8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 43 00 00 00 00 00 00 00 44 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 7A 2E DD E3 22 C0 5E 3B 7F DD BF 0C 16 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 44 00 00 00 00 00 00 00 45 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA CB 1D D5 71 57 C0 5E 3B 77 E3 0C 8B 32 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 45 00 00 00 00 00 00 00 46 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 2C 2F C4 57 17 C0 5E 3B 7D 3D EF 6B 84 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 46 00 00 00 00 00 00 00 47 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 71 FA 77 16 6B C0 5E 3B 91 B5 B7 61 41 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 47 00 00 00 00 00 00 00 48 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 9C 9B B2 BE D6 C0 5E 3B B0 9E 74 84 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 48 00 00 00 00 00 00 00 49 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 9C 9B B2 BE D6 C0 5E 3B B0 9E 74 84 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 49 00 00 00 00 00 00 00 49 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 </t>
-  </si>
-  <si>
-    <t>00 03 55 63</t>
+    <t>Entity ID (8 bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-direction velocity </t>
+  </si>
+  <si>
+    <t>EntityState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 00 1C 17 </t>
+  </si>
+  <si>
+    <t>AutomationResponse</t>
+  </si>
+  <si>
+    <t>MissionCommand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 46 A8 82 44 A0 42 3F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0 5E 3F 67 D5 56 77 B2 </t>
+  </si>
+  <si>
+    <t>00 03 53 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 74 64 98 F0 3E C0 5E 3F 64 7B 68 80 1B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 02 00 00 00 00 00 00 00 03 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 65 BF 07 5C 8C C0 5E 3F 64 E6 8D 8B F6 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 03 00 00 00 00 00 00 00 04 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 58 4B F9 74 81 C0 5E 3F 69 08 5E 52 10 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 04 00 00 00 00 00 00 00 05 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 48 59 5E 32 53 C0 5E 3F 78 67 C2 F1 CA 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 05 00 00 00 00 00 00 00 06 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 B5 6E 2B 3D 14 C0 5E 40 D4 90 B6 47 BE 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 06 00 00 00 00 00 00 00 07 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 AE B9 26 E2 8A C0 5E 40 DD CD 94 1A CC 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 07 00 00 00 00 00 00 00 08 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 A3 C4 54 D1 5A C0 5E 40 E4 B4 88 B9 EB 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 08 00 00 00 00 00 00 00 09 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 96 09 79 17 EF C0 5E 40 E8 58 32 D1 00 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 09 00 00 00 00 00 00 00 0A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 87 61 14 4C C0 C0 5E 40 E8 3B 54 02 33 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0A 00 00 00 00 00 00 00 0B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 79 C3 95 95 FB C0 5E 40 E4 61 CD D9 50 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0B 00 00 00 00 00 00 00 0C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6F 05 8B 07 27 C0 5E 40 DD 50 1C 3B CF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0C 00 00 00 00 00 00 00 0D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 67 3F 52 2D 96 C0 5E 40 CA 80 AF BA EF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0D 00 00 00 00 00 00 00 0E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6E C0 DB 56 DC C0 5E 40 7C 9A F1 E8 B9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0E 00 00 00 00 00 00 00 0F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6B AA FB 77 58 C0 5E 40 75 14 4F A9 E2 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0F 00 00 00 00 00 00 00 10 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 57 83 43 13 C4 C0 5E 40 57 68 54 77 1A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 10 00 00 00 00 00 00 00 11 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 41 B7 7E 6D 5C C0 5E 40 41 3D E2 15 C8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 11 00 00 00 00 00 00 00 12 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 2B 57 F8 B7 8A C0 5E 40 30 C9 94 0F A5 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 12 00 00 00 00 00 00 00 13 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FA E1 35 0E 35 C0 5E 3F EB B8 21 2F 0D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 13 00 00 00 00 00 00 00 14 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF EE 88 C9 28 C0 5E 3F AD A5 7D 31 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 14 00 00 00 00 00 00 00 15 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 1C A7 A6 86 B5 C0 5E 3F 7C 73 19 0E D6 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 15 00 00 00 00 00 00 00 16 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 55 73 6E 47 FE C0 5E 3F 4E 28 29 AB 2A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 16 00 00 00 00 00 00 00 17 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 91 EF 3A 40 7D C0 5E 3F 31 FA D7 F8 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 17 00 00 00 00 00 00 00 18 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 0A 99 E1 B6 E8 C0 5E 3F 14 36 2E 1C B8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 18 00 00 00 00 00 00 00 19 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 1F C8 8A F0 3C C0 5E 3F 0C 14 C9 03 8F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 19 00 00 00 00 00 00 00 1A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 C2 7C 6C D7 38 C0 5E 3E EB E3 1F 4B D0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1A 00 00 00 00 00 00 00 1B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 D5 5D D5 F3 7F C0 5E 3E E5 B9 44 D5 4B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1B 00 00 00 00 00 00 00 1C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 E7 39 3C 77 D7 C0 5E 3E DB 14 37 2E AF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1C 00 00 00 00 00 00 00 1D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 F9 A7 EF 4C B7 C0 5E 3E CB BF 2D B0 35 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1D 00 00 00 00 00 00 00 1E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 09 10 B2 75 AA C0 5E 3E BD 68 C0 50 A4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1E 00 00 00 00 00 00 00 1F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 DF D0 E3 2D 2F C0 5E 3E 89 05 B8 34 27 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 1F 00 00 00 00 00 00 00 20 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 D6 DA 71 21 53 C0 5E 3E 6E 8A 52 F5 17 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 20 00 00 00 00 00 00 00 21 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 CD 91 AB 39 64 C0 5E 3E 74 DC BA D8 F5 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 21 00 00 00 00 00 00 00 22 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 9D E1 2D 43 2F C0 5E 3E 7F C4 56 56 2B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 22 00 00 00 00 00 00 00 23 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 7B D8 CB AF 3E C0 5E 3E 7F BE AB 14 4E 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 23 00 00 00 00 00 00 00 24 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 33 39 E2 83 6C C0 5E 3E 8B 7A A6 3B BE 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 24 00 00 00 00 00 00 00 25 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 EC AE 28 6A 9E C0 5E 3E 86 F4 9E 5D 7D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 25 00 00 00 00 00 00 00 26 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 9A 87 32 4D 9C C0 5E 3E 74 A1 DC DB 58 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 26 00 00 00 00 00 00 00 27 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 67 29 AC 98 0F C0 5E 3E 62 CF B9 94 DC 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 27 00 00 00 00 00 00 00 28 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 38 6B 5E 37 F6 C0 5E 3E 46 91 21 7F B8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 28 00 00 00 00 00 00 00 29 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 16 22 81 20 1A C0 5E 3E 1C 2A 08 0C 1F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 29 00 00 00 00 00 00 00 2A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF 6C F8 CD B2 C0 5E 3D E7 76 E6 77 9F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2A 00 00 00 00 00 00 00 2B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A6 FF BF E3 EC 87 C0 5E 3D 99 B7 DB 1F 74 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2B 00 00 00 00 00 00 00 2C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 1E B3 03 2D 2F C0 5E 3D 5F 4D 45 67 3F 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2C 00 00 00 00 00 00 00 2D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 48 A0 08 48 74 C0 5E 3D 38 89 1A 46 A6 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2D 00 00 00 00 00 00 00 2E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 82 A0 1E 08 A7 C0 5E 3D 11 D1 46 B2 D8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2E 00 00 00 00 00 00 00 2F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 03 0B 1B 06 A3 C0 5E 3C FB F0 4E 6D 13 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 2F 00 00 00 00 00 00 00 30 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 21 FA A4 E1 33 C0 5E 3C FC 08 5C 78 82 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 30 00 00 00 00 00 00 00 31 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 7F C4 EE 6F 65 C0 5E 3C DE 15 82 B9 B4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 31 00 00 00 00 00 00 00 32 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 E1 0C E6 A8 23 C0 5E 3C A2 E2 3C 17 C0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 32 00 00 00 00 00 00 00 33 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 38 92 68 29 D7 C0 5E 3C 78 AC FF 30 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 33 00 00 00 00 00 00 00 34 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 70 13 EB AA 4B C0 5E 3C 62 B0 AB 7B 0A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 34 00 00 00 00 00 00 00 35 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 9D E8 AF B7 5B C0 5E 3C 59 5D 36 68 25 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 35 00 00 00 00 00 00 00 36 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A9 F6 70 DC 1D 73 C0 5E 3C 56 7B 54 75 F0 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 36 00 00 00 00 00 00 00 37 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 83 26 A4 4F 6E C0 5E 3C 66 37 0D C1 1D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 37 00 00 00 00 00 00 00 38 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA AF 49 62 B1 EC C0 5E 3C 86 B9 AB 72 FF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 38 00 00 00 00 00 00 00 39 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA E6 59 92 3E 7C C0 5E 3C F1 D7 6D 0C 3B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 39 00 00 00 00 00 00 00 3A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA EE D4 67 81 69 C0 5E 3C EC B5 A0 DA 28 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3A 00 00 00 00 00 00 00 3B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F7 49 60 7B 1C C0 5E 3C E9 F0 1C 5E C4 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3B 00 00 00 00 00 00 00 3C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F7 73 0E 3A AD C0 5E 3C DC 03 C5 D4 2E 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3C 00 00 00 00 00 00 00 3D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA F4 BB C9 50 D6 C0 5E 3C CC 46 AF B7 09 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3D 00 00 00 00 00 00 00 3E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA EA 2E 6B C0 CF C0 5E 3C B4 72 53 72 FD 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3E 00 00 00 00 00 00 00 3F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA C1 28 4D 2F 56 C0 5E 3C 93 F3 CD 47 1B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 3F 00 00 00 00 00 00 00 40 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 7E 82 25 A6 42 C0 5E 3C 53 8C FF AC B9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 40 00 00 00 00 00 00 00 41 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 18 90 79 49 49 C0 5E 3B FC 3E 1B 37 80 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 41 00 00 00 00 00 00 00 42 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 1D 91 D5 A9 60 C0 5E 3B CD 0F CC E2 9C 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 42 00 00 00 00 00 00 00 43 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 3C 22 AF 05 59 C0 5E 3B 9E A7 F4 65 D8 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 43 00 00 00 00 00 00 00 44 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA 7A 2E DD E3 22 C0 5E 3B 7F DD BF 0C 16 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 44 00 00 00 00 00 00 00 45 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AA CB 1D D5 71 57 C0 5E 3B 77 E3 0C 8B 32 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 45 00 00 00 00 00 00 00 46 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 2C 2F C4 57 17 C0 5E 3B 7D 3D EF 6B 84 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 46 00 00 00 00 00 00 00 47 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 71 FA 77 16 6B C0 5E 3B 91 B5 B7 61 41 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 47 00 00 00 00 00 00 00 48 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 9C 9B B2 BE D6 C0 5E 3B B0 9E 74 84 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 48 00 00 00 00 00 00 00 49 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 AB 9C 9B B2 BE D6 C0 5E 3B B0 9E 74 84 94 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 49 00 00 00 00 00 00 00 49 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00  </t>
+  </si>
+  <si>
+    <t>00 00 00 00 00 00 00 01</t>
+  </si>
+  <si>
+    <t>Mission Command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 66 72 6C 2E 63 6D 61 73 69 2E 4D 69 73 73 69 6F 6E 43 6F 6D 6D 61 6E 64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">36 33 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 00 05 94 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 00 00 00 00 00 00 48 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00 0F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 46 A8 85 38 56 D4 57 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0 5E 3F 69 21 BE 91 4E </t>
+  </si>
+  <si>
+    <t>Waypoints 2-15</t>
+  </si>
+  <si>
+    <t>00 00 A7 D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 77 CD A8 3F 85 C0 5E 3F 64 F2 57 E5 31 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 02 00 00 00 00 00 00 00 03 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 69 28 FD 4A 36 C0 5E 3F 64 78 63 2D DF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 03 00 00 00 00 00 00 00 04 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 5B 42 44 E1 39 C0 5E 3F 67 C4 45 6B 54 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 04 00 00 00 00 00 00 00 05 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 4F F7 E5 13 D3 C0 5E 3F 6E 64 8D 23 95 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 05 00 00 00 00 00 00 00 06 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A8 48 60 61 8B 3A C0 5E 3F 78 6A 06 C2 91 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 06 00 00 00 00 00 00 00 07 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 B5 6D CC C1 6A C0 5E 40 D4 91 69 70 C9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 07 00 00 00 00 00 00 00 08 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 AE B8 81 CF 88 C0 5E 40 DD CE 2A E5 4A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 08 00 00 00 00 00 00 00 09 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 A3 C3 6E 27 F3 C0 5E 40 E4 B4 EB 36 2D 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 09 00 00 00 00 00 00 00 0A 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 96 08 6F DA 27 C0 5E 40 E8 58 53 C1 BC 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0A 00 00 00 00 00 00 00 0B 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 87 60 0C 22 A1 C0 5E 40 E8 3B 2E F9 CC 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0B 00 00 00 00 00 00 00 0C 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 79 C2 B2 02 7D C0 5E 40 E4 61 67 D2 3B 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0C 00 00 00 00 00 00 00 0D 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6F 04 EA A2 1C C0 5E 40 DD 4F 82 ED 3A 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0D 00 00 00 00 00 00 00 0E 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 67 3F 52 2D 96 C0 5E 40 CA 80 AF BA EF 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0E 00 00 00 00 00 00 00 0F 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 01 43 4D 41 53 49 00 00 00 00 00 00 23 00 03 40 46 A7 6E C0 DB 56 DC C0 5E 40 7C 9A F1 E8 B9 44 2F 00 00 00 00 00 01 00 00 00 00 00 00 00 0F 00 00 00 00 00 00 00 10 41 B0 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 01 00 00 00 00 00 00 03 E8 </t>
   </si>
 </sst>
 </file>
@@ -941,7 +851,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -984,6 +894,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -997,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1039,9 +973,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:EF52"/>
+  <dimension ref="A2:BM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,18 +1284,22 @@
     <col min="18" max="18" width="13" customWidth="1"/>
     <col min="20" max="20" width="15" customWidth="1"/>
     <col min="21" max="21" width="13.140625" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" customWidth="1"/>
     <col min="23" max="23" width="14.42578125" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" customWidth="1"/>
     <col min="26" max="26" width="11.5703125" customWidth="1"/>
     <col min="27" max="27" width="10.42578125" customWidth="1"/>
+    <col min="28" max="28" width="13.28515625" customWidth="1"/>
     <col min="29" max="30" width="11.42578125" customWidth="1"/>
     <col min="32" max="32" width="10.42578125" customWidth="1"/>
     <col min="33" max="33" width="10.5703125" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" customWidth="1"/>
+    <col min="36" max="36" width="12.28515625" customWidth="1"/>
     <col min="39" max="39" width="10.7109375" customWidth="1"/>
+    <col min="40" max="40" width="9.85546875" customWidth="1"/>
     <col min="43" max="43" width="11.28515625" customWidth="1"/>
+    <col min="44" max="44" width="13" customWidth="1"/>
     <col min="45" max="45" width="10.42578125" customWidth="1"/>
     <col min="46" max="46" width="10.28515625" customWidth="1"/>
     <col min="48" max="48" width="10.140625" customWidth="1"/>
@@ -2518,13 +2457,13 @@
     <row r="31" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
     </row>
-    <row r="33" spans="1:136" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>145</v>
       </c>
       <c r="R33" s="6"/>
     </row>
-    <row r="34" spans="1:136" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -2553,8 +2492,46 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
-    </row>
-    <row r="35" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="2"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+      <c r="AP34" s="2"/>
+      <c r="AQ34" s="2"/>
+      <c r="AR34" s="2"/>
+      <c r="AS34" s="2"/>
+      <c r="AT34" s="2"/>
+      <c r="AU34" s="2"/>
+      <c r="AV34" s="2"/>
+      <c r="AW34" s="2"/>
+      <c r="AX34" s="2"/>
+      <c r="AY34" s="2"/>
+      <c r="AZ34" s="2"/>
+      <c r="BA34" s="2"/>
+      <c r="BB34" s="2"/>
+      <c r="BC34" s="2"/>
+      <c r="BD34" s="2"/>
+      <c r="BE34" s="2"/>
+      <c r="BF34" s="2"/>
+      <c r="BG34" s="2"/>
+      <c r="BH34" s="2"/>
+      <c r="BI34" s="2"/>
+      <c r="BJ34" s="2"/>
+      <c r="BK34" s="2"/>
+      <c r="BL34" s="2"/>
+      <c r="BM34" s="2"/>
+    </row>
+    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
       <c r="N35" s="5" t="s">
         <v>10</v>
       </c>
@@ -2571,8 +2548,46 @@
       <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
-    </row>
-    <row r="36" spans="1:136" x14ac:dyDescent="0.25">
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="5"/>
+      <c r="AP35" s="5"/>
+      <c r="AQ35" s="5"/>
+      <c r="AR35" s="5"/>
+      <c r="AS35" s="5"/>
+      <c r="AT35" s="5"/>
+      <c r="AU35" s="5"/>
+      <c r="AV35" s="5"/>
+      <c r="AW35" s="5"/>
+      <c r="AX35" s="5"/>
+      <c r="AY35" s="5"/>
+      <c r="AZ35" s="5"/>
+      <c r="BA35" s="5"/>
+      <c r="BB35" s="5"/>
+      <c r="BC35" s="5"/>
+      <c r="BD35" s="5"/>
+      <c r="BE35" s="5"/>
+      <c r="BF35" s="5"/>
+      <c r="BG35" s="5"/>
+      <c r="BH35" s="5"/>
+      <c r="BI35" s="5"/>
+      <c r="BJ35" s="5"/>
+      <c r="BK35" s="5"/>
+      <c r="BL35" s="5"/>
+      <c r="BM35" s="5"/>
+    </row>
+    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
       <c r="P36" s="4" t="s">
         <v>12</v>
       </c>
@@ -2586,69 +2601,160 @@
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
-      <c r="AA36" s="17"/>
-    </row>
-    <row r="37" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="T37" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="4"/>
+      <c r="AC36" s="4"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+      <c r="AH36" s="4"/>
+      <c r="AI36" s="4"/>
+      <c r="AJ36" s="4"/>
+      <c r="AK36" s="4"/>
+      <c r="AL36" s="4"/>
+      <c r="AM36" s="4"/>
+      <c r="AN36" s="4"/>
+      <c r="AO36" s="4"/>
+      <c r="AP36" s="4"/>
+      <c r="AQ36" s="4"/>
+      <c r="AR36" s="4"/>
+      <c r="AS36" s="4"/>
+      <c r="AT36" s="4"/>
+      <c r="AU36" s="4"/>
+      <c r="AV36" s="4"/>
+      <c r="AW36" s="4"/>
+      <c r="AX36" s="4"/>
+      <c r="AY36" s="4"/>
+      <c r="AZ36" s="4"/>
+      <c r="BA36" s="4"/>
+      <c r="BB36" s="4"/>
+      <c r="BC36" s="4"/>
+      <c r="BD36" s="4"/>
+      <c r="BE36" s="4"/>
+      <c r="BF36" s="4"/>
+      <c r="BG36" s="4"/>
+      <c r="BH36" s="4"/>
+      <c r="BI36" s="4"/>
+      <c r="BJ36" s="4"/>
+      <c r="BK36" s="4"/>
+      <c r="BL36" s="4"/>
+    </row>
+    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="P37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-      <c r="BH37" s="9"/>
-      <c r="BI37" s="9"/>
-    </row>
-    <row r="38" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="T38" s="3" t="s">
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
+      <c r="AG37" s="3"/>
+      <c r="AH37" s="3"/>
+      <c r="AI37" s="3"/>
+      <c r="AJ37" s="3"/>
+      <c r="AK37" s="3"/>
+      <c r="AL37" s="3"/>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+      <c r="AU37" s="3"/>
+      <c r="AV37" s="3"/>
+      <c r="AW37" s="3"/>
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="3"/>
+      <c r="AZ37" s="3"/>
+      <c r="BA37" s="3"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+      <c r="BD37" s="3"/>
+      <c r="BE37" s="3"/>
+      <c r="BF37" s="3"/>
+      <c r="BG37" s="3"/>
+      <c r="BH37" s="3"/>
+      <c r="BI37" s="3"/>
+      <c r="BJ37" s="3"/>
+      <c r="BK37" s="3"/>
+      <c r="BL37" s="3"/>
+    </row>
+    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="T38" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="24"/>
+      <c r="Y38" s="24"/>
+      <c r="Z38" s="24"/>
+      <c r="AA38" s="24"/>
+      <c r="AB38" s="24"/>
+      <c r="AC38" s="24"/>
+      <c r="AD38" s="24"/>
+      <c r="AE38" s="24"/>
+      <c r="AF38" s="24"/>
+      <c r="AG38" s="24"/>
+      <c r="AH38" s="24"/>
+      <c r="AI38" s="24"/>
+      <c r="AJ38" s="24"/>
+      <c r="AK38" s="24"/>
+      <c r="AL38" s="24"/>
+      <c r="AM38" s="24"/>
+      <c r="AN38" s="24"/>
+      <c r="AO38" s="24"/>
+      <c r="AP38" s="24"/>
+      <c r="AQ38" s="24"/>
+      <c r="AR38" s="24"/>
+      <c r="AS38" s="24"/>
+      <c r="AT38" s="24"/>
+      <c r="AU38" s="24"/>
+      <c r="AV38" s="24"/>
+      <c r="AW38" s="24"/>
+      <c r="AX38" s="24"/>
+      <c r="AY38" s="24"/>
+      <c r="AZ38" s="24"/>
+      <c r="BA38" s="24"/>
+      <c r="BB38" s="24"/>
+      <c r="BC38" s="24"/>
+      <c r="BD38" s="24"/>
+      <c r="BE38" s="24"/>
+      <c r="BF38" s="24"/>
+      <c r="BG38" s="24"/>
+      <c r="BH38" s="24"/>
+    </row>
+    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+      <c r="AA39" s="17"/>
+      <c r="AB39" s="17"/>
+      <c r="AC39" s="17"/>
+      <c r="AD39" s="17"/>
+      <c r="AE39" s="17"/>
+      <c r="AF39" s="17"/>
+      <c r="AG39" s="17"/>
+      <c r="AH39" s="17"/>
+      <c r="AI39" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="3"/>
-      <c r="AD38" s="3"/>
-      <c r="AE38" s="3"/>
-      <c r="AF38" s="3"/>
-      <c r="AG38" s="3"/>
-      <c r="AH38" s="3"/>
-      <c r="AI38" s="3"/>
-      <c r="AJ38" s="3"/>
-      <c r="AK38" s="3"/>
-      <c r="AL38" s="3"/>
-      <c r="AM38" s="3"/>
-      <c r="AN38" s="3"/>
-      <c r="AO38" s="3"/>
-      <c r="AP38" s="3"/>
-      <c r="AQ38" s="3"/>
-      <c r="AR38" s="3"/>
-      <c r="AS38" s="3"/>
-      <c r="BH38" s="9"/>
-      <c r="BI38" s="9"/>
-      <c r="BY38" t="s">
-        <v>147</v>
-      </c>
-      <c r="DE38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AI39" s="20" t="s">
-        <v>149</v>
       </c>
       <c r="AJ39" s="20"/>
       <c r="AK39" s="20"/>
@@ -2657,89 +2763,28 @@
       <c r="AN39" s="20"/>
       <c r="AO39" s="20"/>
       <c r="AP39" s="20"/>
-      <c r="AT39" t="s">
-        <v>150</v>
-      </c>
-      <c r="AX39" t="s">
-        <v>151</v>
-      </c>
-      <c r="AZ39" t="s">
-        <v>152</v>
-      </c>
-      <c r="BH39" t="s">
-        <v>150</v>
-      </c>
-      <c r="BI39" s="9"/>
-      <c r="BL39" t="s">
-        <v>153</v>
-      </c>
-      <c r="BP39" t="s">
-        <v>151</v>
-      </c>
-      <c r="BR39" t="s">
-        <v>154</v>
-      </c>
-      <c r="BV39" t="s">
-        <v>153</v>
-      </c>
-      <c r="BY39" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="BZ39" s="20"/>
-      <c r="CA39" s="20"/>
-      <c r="CB39" s="20"/>
-      <c r="CC39" s="20"/>
-      <c r="CD39" s="20"/>
-      <c r="CE39" s="20"/>
-      <c r="CF39" s="20"/>
-      <c r="CG39" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="CH39" s="20"/>
-      <c r="CI39" s="20"/>
-      <c r="CJ39" s="20"/>
-      <c r="CK39" s="20"/>
-      <c r="CL39" s="20"/>
-      <c r="CM39" s="20"/>
-      <c r="CN39" s="20"/>
-      <c r="CO39" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="CP39" s="20"/>
-      <c r="CQ39" s="20"/>
-      <c r="CR39" s="20"/>
-      <c r="CS39" s="20"/>
-      <c r="CT39" s="20"/>
-      <c r="CU39" s="20"/>
-      <c r="CV39" s="20"/>
-      <c r="CW39" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="CX39" s="20"/>
-      <c r="CY39" s="20"/>
-      <c r="CZ39" s="20"/>
-      <c r="DA39" s="20"/>
-      <c r="DB39" s="20"/>
-      <c r="DC39" s="20"/>
-      <c r="DD39" s="20"/>
-      <c r="DE39" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="DF39" s="20"/>
-      <c r="DG39" s="20"/>
-      <c r="DH39" s="20"/>
-      <c r="DI39" s="20"/>
-      <c r="DJ39" s="20"/>
-      <c r="DK39" s="20"/>
-      <c r="DL39" s="20"/>
-      <c r="DT39" t="s">
-        <v>155</v>
-      </c>
-      <c r="EB39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:136" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="AQ39" s="17"/>
+      <c r="AR39" s="17"/>
+      <c r="AS39" s="17"/>
+      <c r="AT39" s="17"/>
+      <c r="AU39" s="17"/>
+      <c r="AV39" s="17"/>
+      <c r="AW39" s="17"/>
+      <c r="AX39" s="17"/>
+      <c r="AY39" s="17"/>
+      <c r="AZ39" s="17"/>
+      <c r="BA39" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="BB39" s="21"/>
+      <c r="BC39" s="21"/>
+      <c r="BD39" s="21"/>
+      <c r="BE39" s="21"/>
+      <c r="BF39" s="21"/>
+      <c r="BG39" s="21"/>
+      <c r="BH39" s="21"/>
+    </row>
+    <row r="40" spans="1:65" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>4</v>
       </c>
@@ -2781,49 +2826,49 @@
         <v>83</v>
       </c>
       <c r="T40" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="U40" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="V40" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="W40" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="X40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y40" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z40" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA40" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB40" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC40" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD40" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="U40" s="9" t="s">
+      <c r="AE40" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="V40" s="9" t="s">
+      <c r="AF40" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="W40" s="9" t="s">
+      <c r="AG40" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="X40" s="9" t="s">
+      <c r="AH40" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="Y40" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z40" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA40" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB40" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC40" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD40" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE40" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="AF40" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="AG40" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH40" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="AI40" s="9" t="s">
         <v>108</v>
@@ -2850,306 +2895,93 @@
         <v>115</v>
       </c>
       <c r="AQ40" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR40" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="AS40" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AT40" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="AU40" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="AV40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW40" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AR40" s="9" t="s">
+      <c r="AX40" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="AS40" s="9" t="s">
+      <c r="AY40" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AT40" s="9" t="s">
+      <c r="AZ40" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BA40" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="AU40" s="9" t="s">
+      <c r="BB40" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="AV40" s="9" t="s">
+      <c r="BC40" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="AW40" s="9" t="s">
+      <c r="BD40" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AX40" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="AY40" s="9" t="s">
+      <c r="BE40" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF40" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="BG40" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="BH40" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="BI40" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="AZ40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="BA40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="BB40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="BD40" s="9" t="s">
+      <c r="BJ40" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="BE40" s="9" t="s">
+      <c r="BK40" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="BF40" s="9" t="s">
+      <c r="BL40" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="BG40" s="9" t="s">
+      <c r="BM40" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="BH40" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="BI40" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="BJ40" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="BK40" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="BL40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="BM40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="BN40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="BO40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="BP40" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="BQ40" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="BR40" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="BS40" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="BT40" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="BU40" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="BV40" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="BW40" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="BX40" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="BY40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="BZ40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="CA40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="CB40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="CC40" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="CD40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="CE40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="CF40" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="CG40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="CH40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="CI40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="CJ40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="CK40" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="CL40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="CM40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="CN40" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="CO40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="CP40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="CQ40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="CR40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="CS40" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="CT40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="CU40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="CV40" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="CW40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="CX40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="CY40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="CZ40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="DA40" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="DB40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="DC40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="DD40" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="DE40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="DF40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="DG40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="DH40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="DI40" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="DJ40" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="DK40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="DL40" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="DM40" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="DN40" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="DO40" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="DP40" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="DQ40" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="DR40" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="DS40" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="DT40" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="DU40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="DV40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="DW40" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="DX40" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="DY40" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="DZ40" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="EA40" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="EB40" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="EC40" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="ED40" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="EE40" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="EF40" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:136" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="E41" t="s">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G41" t="s">
         <v>2</v>
@@ -3176,7 +3008,7 @@
         <v>3</v>
       </c>
       <c r="O41" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="P41" s="10" t="s">
         <v>18</v>
@@ -3185,7 +3017,7 @@
         <v>16</v>
       </c>
       <c r="R41" s="10" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="S41" s="10" t="s">
         <v>20</v>
@@ -3194,33 +3026,13 @@
       <c r="AJ41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="BY41" s="10"/>
-      <c r="BZ41" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="CG41" s="10"/>
-      <c r="CH41" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="CO41" s="10"/>
-      <c r="CP41" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="CW41" s="10"/>
-      <c r="CX41" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="DE41" s="10"/>
-      <c r="DF41" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:136" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:65" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="C42" s="7">
         <v>24</v>
@@ -3232,25 +3044,25 @@
         <v>47</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>47</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="K42" s="7" t="s">
         <v>47</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="M42" s="7">
         <v>24</v>
@@ -3259,7 +3071,7 @@
         <v>125</v>
       </c>
       <c r="O42" s="7" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="P42" s="10" t="s">
         <v>30</v>
@@ -3268,16 +3080,16 @@
         <v>56</v>
       </c>
       <c r="R42" s="7" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="S42" s="10" t="s">
         <v>32</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="U42" s="7" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="V42" s="7" t="s">
         <v>132</v>
@@ -3295,28 +3107,28 @@
         <v>132</v>
       </c>
       <c r="AA42" s="7" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AB42" s="7" t="s">
         <v>132</v>
       </c>
       <c r="AC42" s="7" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AD42" s="7" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AE42" s="7" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="AF42" s="7" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AG42" s="7" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AH42" s="7" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AI42" s="10" t="s">
         <v>30</v>
@@ -3331,768 +3143,1132 @@
         <v>76</v>
       </c>
       <c r="AM42" s="7" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="AN42" s="7" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="AO42" s="7" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="AP42" s="7" t="s">
         <v>142</v>
       </c>
       <c r="AQ42" s="7" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="AR42" s="7" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="AS42" s="7" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="AT42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AU42" t="s">
-        <v>56</v>
+        <v>73</v>
+      </c>
+      <c r="AU42" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="AV42" s="7" t="s">
-        <v>225</v>
+        <v>78</v>
       </c>
       <c r="AW42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX42" s="7" t="s">
-        <v>226</v>
+        <v>36</v>
       </c>
       <c r="AY42" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH42" s="7" t="s">
-        <v>78</v>
+        <v>208</v>
+      </c>
+      <c r="AZ42" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="BI42" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="BJ42" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="BJ42" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="BK42" s="7" t="s">
         <v>72</v>
       </c>
       <c r="BL42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="BM42" t="s">
-        <v>56</v>
-      </c>
-      <c r="BN42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="BM42" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:65" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="AI43" s="10"/>
+    </row>
+    <row r="44" spans="1:65" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="AI44" s="10"/>
+    </row>
+    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2"/>
+      <c r="AJ47" s="2"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="2"/>
+      <c r="AM47" s="2"/>
+      <c r="AN47" s="2"/>
+      <c r="AO47" s="2"/>
+      <c r="AP47" s="2"/>
+      <c r="AQ47" s="2"/>
+      <c r="AR47" s="2"/>
+      <c r="AS47" s="2"/>
+      <c r="AT47" s="2"/>
+      <c r="AU47" s="2"/>
+      <c r="AV47" s="2"/>
+      <c r="AW47" s="2"/>
+      <c r="AX47" s="2"/>
+      <c r="AY47" s="2"/>
+      <c r="AZ47" s="17"/>
+      <c r="BA47" s="17"/>
+      <c r="BB47" s="17"/>
+      <c r="BC47" s="17"/>
+    </row>
+    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="N48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="5"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="5"/>
+      <c r="AQ48" s="5"/>
+      <c r="AR48" s="5"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="5"/>
+      <c r="AU48" s="5"/>
+      <c r="AV48" s="5"/>
+      <c r="AW48" s="5"/>
+      <c r="AX48" s="5"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="17"/>
+      <c r="BA48" s="17"/>
+      <c r="BB48" s="17"/>
+      <c r="BC48" s="17"/>
+    </row>
+    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="P49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="4"/>
+      <c r="AI49" s="4"/>
+      <c r="AJ49" s="4"/>
+      <c r="AK49" s="4"/>
+      <c r="AL49" s="4"/>
+      <c r="AM49" s="4"/>
+      <c r="AN49" s="4"/>
+      <c r="AO49" s="4"/>
+      <c r="AP49" s="4"/>
+      <c r="AQ49" s="4"/>
+      <c r="AR49" s="4"/>
+      <c r="AS49" s="4"/>
+      <c r="AT49" s="4"/>
+      <c r="AU49" s="4"/>
+      <c r="AV49" s="4"/>
+      <c r="AW49" s="4"/>
+      <c r="AX49" s="4"/>
+      <c r="AY49" s="17"/>
+      <c r="AZ49" s="17"/>
+      <c r="BA49" s="17"/>
+      <c r="BB49" s="17"/>
+      <c r="BC49" s="17"/>
+    </row>
+    <row r="50" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="P50" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AD50" s="3"/>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3"/>
+      <c r="AL50" s="3"/>
+      <c r="AM50" s="3"/>
+      <c r="AN50" s="3"/>
+      <c r="AO50" s="3"/>
+      <c r="AP50" s="3"/>
+      <c r="AQ50" s="3"/>
+      <c r="AR50" s="3"/>
+      <c r="AS50" s="3"/>
+      <c r="AT50" s="3"/>
+      <c r="AU50" s="3"/>
+      <c r="AV50" s="3"/>
+      <c r="AW50" s="3"/>
+      <c r="AX50" s="3"/>
+    </row>
+    <row r="51" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U51" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="V51" s="24"/>
+      <c r="W51" s="24"/>
+      <c r="X51" s="24"/>
+      <c r="Y51" s="24"/>
+      <c r="Z51" s="24"/>
+      <c r="AA51" s="24"/>
+      <c r="AB51" s="24"/>
+      <c r="AC51" s="24"/>
+      <c r="AD51" s="24"/>
+      <c r="AE51" s="24"/>
+      <c r="AF51" s="24"/>
+      <c r="AG51" s="24"/>
+      <c r="AH51" s="24"/>
+      <c r="AI51" s="24"/>
+      <c r="AJ51" s="24"/>
+      <c r="AK51" s="24"/>
+      <c r="AL51" s="24"/>
+      <c r="AM51" s="24"/>
+      <c r="AN51" s="24"/>
+      <c r="AO51" s="24"/>
+      <c r="AP51" s="24"/>
+      <c r="AQ51" s="24"/>
+      <c r="AR51" s="24"/>
+      <c r="AS51" s="24"/>
+      <c r="AT51" s="24"/>
+      <c r="AU51" s="24"/>
+      <c r="AV51" s="24"/>
+    </row>
+    <row r="52" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y52" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z52" s="22"/>
+      <c r="AA52" s="22"/>
+      <c r="AC52" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD52" s="23"/>
+      <c r="AE52" s="23"/>
+      <c r="AF52" s="23"/>
+      <c r="AG52" s="23"/>
+      <c r="AH52" s="23"/>
+      <c r="AI52" s="23"/>
+      <c r="AJ52" s="23"/>
+      <c r="AK52" s="23"/>
+      <c r="AL52" s="23"/>
+      <c r="AM52" s="23"/>
+      <c r="AN52" s="23"/>
+      <c r="AO52" s="23"/>
+      <c r="AP52" s="23"/>
+      <c r="AQ52" s="23"/>
+      <c r="AR52" s="23"/>
+      <c r="AS52" s="23"/>
+      <c r="AT52" s="23"/>
+    </row>
+    <row r="53" spans="1:55" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AG53" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH53" s="20"/>
+      <c r="AI53" s="20"/>
+      <c r="AJ53" s="20"/>
+    </row>
+    <row r="54" spans="1:55" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q54" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="R54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="S54" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T54" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="U54" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="V54" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="W54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="X54" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y54" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z54" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA54" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB54" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC54" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD54" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF54" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG54" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH54" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI54" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ54" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK54" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AL54" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AM54" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AN54" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AO54" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP54" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AQ54" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AR54" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AS54" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AT54" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AU54" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="AV54" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW54" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX54" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AY54" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="M55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N55" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O55" s="10"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="10"/>
+      <c r="V55" s="10"/>
+      <c r="W55" s="14"/>
+      <c r="X55" s="10"/>
+      <c r="Y55" s="16"/>
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="15"/>
+    </row>
+    <row r="56" spans="1:55" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="N56" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="R56" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="T56" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="U56" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="V56" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="W56" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="X56" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y56" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z56" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA56" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB56" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC56" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD56" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE56" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF56" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG56" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH56" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AI56" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="AJ56" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK56" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="AL56" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="AM56" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AN56" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO56" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP56" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ56" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR56" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS56" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT56" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU56" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AV56" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="AW56" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX56" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY56" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="2"/>
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+      <c r="X61" s="2"/>
+      <c r="Y61" s="2"/>
+      <c r="Z61" s="2"/>
+      <c r="AA61" s="2"/>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="2"/>
+      <c r="AE61" s="2"/>
+      <c r="AF61" s="2"/>
+      <c r="AG61" s="2"/>
+      <c r="AH61" s="2"/>
+      <c r="AI61" s="2"/>
+      <c r="AJ61" s="2"/>
+      <c r="AK61" s="2"/>
+      <c r="AL61" s="2"/>
+      <c r="AM61" s="2"/>
+      <c r="AN61" s="2"/>
+      <c r="AO61" s="2"/>
+      <c r="AP61" s="2"/>
+      <c r="AQ61" s="2"/>
+      <c r="AR61" s="2"/>
+      <c r="AS61" s="2"/>
+      <c r="AT61" s="2"/>
+    </row>
+    <row r="62" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="N62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="5"/>
+      <c r="AB62" s="5"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="5"/>
+      <c r="AE62" s="5"/>
+      <c r="AF62" s="5"/>
+      <c r="AG62" s="5"/>
+      <c r="AH62" s="5"/>
+      <c r="AI62" s="5"/>
+      <c r="AJ62" s="5"/>
+      <c r="AK62" s="5"/>
+      <c r="AL62" s="5"/>
+      <c r="AM62" s="5"/>
+      <c r="AN62" s="5"/>
+      <c r="AO62" s="5"/>
+      <c r="AP62" s="5"/>
+      <c r="AQ62" s="5"/>
+      <c r="AR62" s="5"/>
+      <c r="AS62" s="5"/>
+      <c r="AT62" s="5"/>
+    </row>
+    <row r="63" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="P63" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="4"/>
+      <c r="X63" s="4"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="4"/>
+      <c r="AA63" s="4"/>
+      <c r="AB63" s="4"/>
+      <c r="AC63" s="4"/>
+      <c r="AD63" s="4"/>
+      <c r="AE63" s="4"/>
+      <c r="AF63" s="4"/>
+      <c r="AG63" s="4"/>
+      <c r="AH63" s="4"/>
+      <c r="AI63" s="4"/>
+      <c r="AJ63" s="4"/>
+      <c r="AK63" s="4"/>
+      <c r="AL63" s="4"/>
+      <c r="AM63" s="4"/>
+      <c r="AN63" s="4"/>
+      <c r="AO63" s="4"/>
+      <c r="AP63" s="4"/>
+      <c r="AQ63" s="4"/>
+      <c r="AR63" s="4"/>
+      <c r="AS63" s="4"/>
+    </row>
+    <row r="64" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="P64" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3"/>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3"/>
+      <c r="AC64" s="3"/>
+      <c r="AD64" s="3"/>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3"/>
+      <c r="AL64" s="3"/>
+      <c r="AM64" s="3"/>
+      <c r="AN64" s="3"/>
+      <c r="AO64" s="3"/>
+      <c r="AP64" s="3"/>
+      <c r="AQ64" s="3"/>
+      <c r="AR64" s="3"/>
+      <c r="AS64" s="3"/>
+    </row>
+    <row r="65" spans="1:46" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T65" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="U65" s="22"/>
+      <c r="V65" s="22"/>
+      <c r="W65" s="22"/>
+      <c r="Y65" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="Z65" s="18"/>
+      <c r="AA65" s="18"/>
+      <c r="AB65" s="18"/>
+      <c r="AC65" s="18"/>
+      <c r="AD65" s="18"/>
+      <c r="AE65" s="18"/>
+      <c r="AF65" s="18"/>
+      <c r="AG65" s="18"/>
+      <c r="AH65" s="18"/>
+      <c r="AI65" s="18"/>
+      <c r="AJ65" s="18"/>
+      <c r="AK65" s="18"/>
+      <c r="AL65" s="18"/>
+      <c r="AM65" s="18"/>
+      <c r="AN65" s="18"/>
+      <c r="AO65" s="18"/>
+      <c r="AP65" s="18"/>
+      <c r="AQ65" s="18"/>
+    </row>
+    <row r="66" spans="1:46" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC66" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="AD66" s="20"/>
+      <c r="AE66" s="20"/>
+      <c r="AF66" s="20"/>
+    </row>
+    <row r="67" spans="1:46" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O67" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P67" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q67" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="R67" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="S67" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T67" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="U67" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="V67" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="W67" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="X67" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y67" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z67" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA67" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB67" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD67" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE67" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF67" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG67" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AH67" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI67" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ67" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AK67" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AL67" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AM67" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="AN67" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="BO42" s="7" t="s">
+      <c r="AO67" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP67" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ67" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR67" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="AS67" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="AT67" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" s="7">
+        <v>24</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L68" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="M68" s="7">
+        <v>24</v>
+      </c>
+      <c r="N68" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O68" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="P68" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q68" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="R68" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="S68" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="BP42" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="BQ42" s="7" t="s">
+      <c r="T68" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="U68" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="V68" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="BR42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="BS42" s="7" t="s">
+      <c r="W68" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="X68" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y68" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z68" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA68" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB68" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC68" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD68" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE68" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF68" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG68" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="AH68" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="AI68" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ68" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="BT42" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="BU42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV42" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="BW42" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="BX42" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="BY42" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="BZ42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="CA42" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="CB42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="CC42" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="CD42" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="CE42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="CF42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="CG42" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="CH42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="CI42" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="CJ42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="CK42" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="CL42" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="CM42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="CN42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="CO42" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="CP42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="CQ42" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="CR42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="CS42" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="CT42" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="CU42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="CV42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="CW42" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="CX42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="CY42" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="CZ42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="DA42" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="DB42" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="DC42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="DD42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="DE42" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="DF42" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="DG42" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="DH42" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="DI42" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="DJ42" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="DK42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="DL42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="DM42" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="DN42" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="DO42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="DP42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR42" s="7" t="s">
+      <c r="AK68" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL68" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM68" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO68" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP68" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AQ68" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR68" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="AS68" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="DS42" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="EB42" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="EC42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="ED42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="EE42" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="EF42" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="45" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
-      <c r="Z46" s="2"/>
-      <c r="AA46" s="2"/>
-    </row>
-    <row r="47" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="N47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5"/>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="5"/>
-    </row>
-    <row r="48" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="P48" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="4"/>
-      <c r="AA48" s="17"/>
-    </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="T49" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="3"/>
-      <c r="Y49" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z49" s="3"/>
-      <c r="AA49" s="3"/>
-      <c r="AF49" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="AG49" s="20"/>
-      <c r="AH49" t="s">
-        <v>250</v>
-      </c>
-      <c r="AI49" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="AJ49" s="20"/>
-      <c r="AK49" s="20"/>
-      <c r="AL49" s="3"/>
-      <c r="AN49" t="s">
-        <v>252</v>
-      </c>
-      <c r="AR49" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="50" spans="1:66" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P50" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q50" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="R50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="S50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="T50" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="U50" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="V50" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="W50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="X50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y50" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z50" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="AA50" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB50" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC50" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF50" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="AG50" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="AH50" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AI50" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="AJ50" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="AK50" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="AL50" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="AM50" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="AN50" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO50" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP50" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR50" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="AS50" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AT50" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="AU50" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="AV50" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW50" s="9" t="s">
+      <c r="AT68" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="AX50" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="AY50" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="AZ50" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="BA50" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="BB50" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="BC50" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="BD50" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="BE50" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="BF50" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="BG50" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="BH50" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="BI50" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="BJ50" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL50" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="BN50" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:66" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="J51" s="10" t="s">
-        <v>280</v>
-      </c>
-      <c r="K51" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L51" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="M51" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N51" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="10"/>
-      <c r="T51" s="10"/>
-      <c r="U51" s="10"/>
-      <c r="V51" s="10"/>
-      <c r="W51" s="14"/>
-      <c r="X51" s="10"/>
-      <c r="Y51" s="16"/>
-      <c r="Z51" s="16"/>
-      <c r="AA51" s="15"/>
-    </row>
-    <row r="52" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>282</v>
-      </c>
-      <c r="C52">
-        <v>24</v>
-      </c>
-      <c r="D52" t="s">
-        <v>121</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="K52" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="M52" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="N52" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="O52" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="P52" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q52" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="R52" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="S52" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="T52" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="U52" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="V52" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="W52" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="X52" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y52" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="Z52" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA52" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB52" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC52" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD52" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="AE52" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF52" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG52" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH52" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="AI52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AJ52" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="AK52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AL52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AM52" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="AN52" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="AO52" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP52" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="AQ52" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR52" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="AS52" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="AT52" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="AU52" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="AV52" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="AW52" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="AX52" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="AY52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AZ52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="BA52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="BB52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="BD52" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="BE52" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH52" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="BI52" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="BJ52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="BL52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="BN52" s="10" t="s">
-        <v>297</v>
-      </c>
-    </row>
+    </row>
+    <row r="69" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating examples to work with new BriefCASE enhancements
</commit_message>
<xml_diff>
--- a/TA2/lmcp-message-format/LMCP messages.xlsx
+++ b/TA2/lmcp-message-format/LMCP messages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="431">
   <si>
     <t>$</t>
   </si>
@@ -1306,6 +1306,18 @@
   </si>
   <si>
     <t>00 48 91 00</t>
+  </si>
+  <si>
+    <t>00 00 04 EB</t>
+  </si>
+  <si>
+    <t>00 0D</t>
+  </si>
+  <si>
+    <t>40 46 A7 CE D9 16 82 76</t>
+  </si>
+  <si>
+    <t>C0 5E 3D C2 8F 5C 22 AE</t>
   </si>
 </sst>
 </file>
@@ -1732,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BE85"/>
+  <dimension ref="A2:BE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ65" sqref="AZ65"/>
+    <sheetView tabSelected="1" topLeftCell="AA53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK66" sqref="AK66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5797,462 +5809,439 @@
         <v>426</v>
       </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>416</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" t="s">
+        <v>416</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K66" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L66" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="M66" s="7">
+        <v>24</v>
+      </c>
+      <c r="N66" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="O66" t="s">
+        <v>427</v>
+      </c>
+      <c r="P66" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q66" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R66" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="S66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="T66" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="U66" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="V66" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="W66" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="X66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y66" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z66" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA66" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB66" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC66" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="AD66" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE66" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF66" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="AG66" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH66" t="s">
+        <v>429</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>430</v>
+      </c>
+      <c r="AJ66" t="s">
+        <v>263</v>
+      </c>
+      <c r="AP66" s="15"/>
+      <c r="AQ66" s="15"/>
+      <c r="AR66" s="15"/>
+      <c r="AS66" s="15"/>
+      <c r="AT66" s="15"/>
+      <c r="AU66" s="15"/>
+    </row>
+    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
-      <c r="S68" s="2"/>
-      <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
-      <c r="W68" s="2"/>
-      <c r="X68" s="2"/>
-      <c r="Y68" s="2"/>
-      <c r="Z68" s="2"/>
-      <c r="AA68" s="2"/>
-      <c r="AB68" s="2"/>
-      <c r="AC68" s="2"/>
-      <c r="AD68" s="2"/>
-      <c r="AE68" s="2"/>
-      <c r="AF68" s="2"/>
-      <c r="AG68" s="2"/>
-      <c r="AH68" s="2"/>
-      <c r="AI68" s="2"/>
-      <c r="AJ68" s="2"/>
-      <c r="AK68" s="2"/>
-      <c r="AL68" s="2"/>
-      <c r="AM68" s="2"/>
-      <c r="AN68" s="2"/>
-      <c r="AO68" s="2"/>
-      <c r="AP68" s="2"/>
-      <c r="AQ68" s="2"/>
-      <c r="AR68" s="2"/>
-      <c r="AS68" s="2"/>
-      <c r="AT68" s="2"/>
-    </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="N69" s="5" t="s">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+      <c r="X69" s="2"/>
+      <c r="Y69" s="2"/>
+      <c r="Z69" s="2"/>
+      <c r="AA69" s="2"/>
+      <c r="AB69" s="2"/>
+      <c r="AC69" s="2"/>
+      <c r="AD69" s="2"/>
+      <c r="AE69" s="2"/>
+      <c r="AF69" s="2"/>
+      <c r="AG69" s="2"/>
+      <c r="AH69" s="2"/>
+      <c r="AI69" s="2"/>
+      <c r="AJ69" s="2"/>
+      <c r="AK69" s="2"/>
+      <c r="AL69" s="2"/>
+      <c r="AM69" s="2"/>
+      <c r="AN69" s="2"/>
+      <c r="AO69" s="2"/>
+      <c r="AP69" s="2"/>
+      <c r="AQ69" s="2"/>
+      <c r="AR69" s="2"/>
+      <c r="AS69" s="2"/>
+      <c r="AT69" s="2"/>
+    </row>
+    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="N70" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
-      <c r="Z69" s="5"/>
-      <c r="AA69" s="5"/>
-      <c r="AB69" s="5"/>
-      <c r="AC69" s="5"/>
-      <c r="AD69" s="5"/>
-      <c r="AE69" s="5"/>
-      <c r="AF69" s="5"/>
-      <c r="AG69" s="5"/>
-      <c r="AH69" s="5"/>
-      <c r="AI69" s="5"/>
-      <c r="AJ69" s="5"/>
-      <c r="AK69" s="5"/>
-      <c r="AL69" s="5"/>
-      <c r="AM69" s="5"/>
-      <c r="AN69" s="5"/>
-      <c r="AO69" s="5"/>
-      <c r="AP69" s="5"/>
-      <c r="AQ69" s="5"/>
-      <c r="AR69" s="5"/>
-      <c r="AS69" s="5"/>
-      <c r="AT69" s="5"/>
-    </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="P70" s="4" t="s">
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="5"/>
+      <c r="R70" s="5"/>
+      <c r="S70" s="5"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="5"/>
+      <c r="V70" s="5"/>
+      <c r="W70" s="5"/>
+      <c r="X70" s="5"/>
+      <c r="Y70" s="5"/>
+      <c r="Z70" s="5"/>
+      <c r="AA70" s="5"/>
+      <c r="AB70" s="5"/>
+      <c r="AC70" s="5"/>
+      <c r="AD70" s="5"/>
+      <c r="AE70" s="5"/>
+      <c r="AF70" s="5"/>
+      <c r="AG70" s="5"/>
+      <c r="AH70" s="5"/>
+      <c r="AI70" s="5"/>
+      <c r="AJ70" s="5"/>
+      <c r="AK70" s="5"/>
+      <c r="AL70" s="5"/>
+      <c r="AM70" s="5"/>
+      <c r="AN70" s="5"/>
+      <c r="AO70" s="5"/>
+      <c r="AP70" s="5"/>
+      <c r="AQ70" s="5"/>
+      <c r="AR70" s="5"/>
+      <c r="AS70" s="5"/>
+      <c r="AT70" s="5"/>
+    </row>
+    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="P71" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
-      <c r="U70" s="4"/>
-      <c r="V70" s="4"/>
-      <c r="W70" s="4"/>
-      <c r="X70" s="4"/>
-      <c r="Y70" s="4"/>
-      <c r="Z70" s="4"/>
-      <c r="AA70" s="4"/>
-      <c r="AB70" s="4"/>
-      <c r="AC70" s="4"/>
-      <c r="AD70" s="4"/>
-      <c r="AE70" s="4"/>
-      <c r="AF70" s="4"/>
-      <c r="AG70" s="4"/>
-      <c r="AH70" s="4"/>
-      <c r="AI70" s="4"/>
-      <c r="AJ70" s="4"/>
-      <c r="AK70" s="4"/>
-      <c r="AL70" s="4"/>
-      <c r="AM70" s="4"/>
-      <c r="AN70" s="4"/>
-      <c r="AO70" s="4"/>
-      <c r="AP70" s="4"/>
-      <c r="AQ70" s="4"/>
-      <c r="AR70" s="4"/>
-      <c r="AS70" s="4"/>
-    </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="P71" s="3" t="s">
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
+      <c r="Y71" s="4"/>
+      <c r="Z71" s="4"/>
+      <c r="AA71" s="4"/>
+      <c r="AB71" s="4"/>
+      <c r="AC71" s="4"/>
+      <c r="AD71" s="4"/>
+      <c r="AE71" s="4"/>
+      <c r="AF71" s="4"/>
+      <c r="AG71" s="4"/>
+      <c r="AH71" s="4"/>
+      <c r="AI71" s="4"/>
+      <c r="AJ71" s="4"/>
+      <c r="AK71" s="4"/>
+      <c r="AL71" s="4"/>
+      <c r="AM71" s="4"/>
+      <c r="AN71" s="4"/>
+      <c r="AO71" s="4"/>
+      <c r="AP71" s="4"/>
+      <c r="AQ71" s="4"/>
+      <c r="AR71" s="4"/>
+      <c r="AS71" s="4"/>
+    </row>
+    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="P72" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="Q71" s="3"/>
-      <c r="R71" s="3"/>
-      <c r="S71" s="3"/>
-      <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
-      <c r="W71" s="3"/>
-      <c r="X71" s="3"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AA71" s="3"/>
-      <c r="AB71" s="3"/>
-      <c r="AC71" s="3"/>
-      <c r="AD71" s="3"/>
-      <c r="AE71" s="3"/>
-      <c r="AF71" s="3"/>
-      <c r="AG71" s="3"/>
-      <c r="AH71" s="3"/>
-      <c r="AI71" s="3"/>
-      <c r="AJ71" s="3"/>
-      <c r="AK71" s="3"/>
-      <c r="AL71" s="3"/>
-      <c r="AM71" s="3"/>
-      <c r="AN71" s="3"/>
-      <c r="AO71" s="3"/>
-      <c r="AP71" s="3"/>
-      <c r="AQ71" s="3"/>
-      <c r="AR71" s="3"/>
-      <c r="AS71" s="3"/>
-    </row>
-    <row r="72" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="T72" s="21" t="s">
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+      <c r="X72" s="3"/>
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="3"/>
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="3"/>
+      <c r="AC72" s="3"/>
+      <c r="AD72" s="3"/>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="3"/>
+      <c r="AG72" s="3"/>
+      <c r="AH72" s="3"/>
+      <c r="AI72" s="3"/>
+      <c r="AJ72" s="3"/>
+      <c r="AK72" s="3"/>
+      <c r="AL72" s="3"/>
+      <c r="AM72" s="3"/>
+      <c r="AN72" s="3"/>
+      <c r="AO72" s="3"/>
+      <c r="AP72" s="3"/>
+      <c r="AQ72" s="3"/>
+      <c r="AR72" s="3"/>
+      <c r="AS72" s="3"/>
+    </row>
+    <row r="73" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T73" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="U72" s="21"/>
-      <c r="V72" s="21"/>
-      <c r="W72" s="21"/>
-      <c r="Y72" s="18" t="s">
+      <c r="U73" s="21"/>
+      <c r="V73" s="21"/>
+      <c r="W73" s="21"/>
+      <c r="Y73" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="Z72" s="18"/>
-      <c r="AA72" s="18"/>
-      <c r="AB72" s="18"/>
-      <c r="AC72" s="18"/>
-      <c r="AD72" s="18"/>
-      <c r="AE72" s="18"/>
-      <c r="AF72" s="18"/>
-      <c r="AG72" s="18"/>
-      <c r="AH72" s="18"/>
-      <c r="AI72" s="18"/>
-      <c r="AJ72" s="18"/>
-      <c r="AK72" s="18"/>
-      <c r="AL72" s="18"/>
-      <c r="AM72" s="18"/>
-      <c r="AN72" s="18"/>
-      <c r="AO72" s="18"/>
-      <c r="AP72" s="18"/>
-      <c r="AQ72" s="18"/>
-    </row>
-    <row r="73" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="AC73" s="20" t="s">
+      <c r="Z73" s="18"/>
+      <c r="AA73" s="18"/>
+      <c r="AB73" s="18"/>
+      <c r="AC73" s="18"/>
+      <c r="AD73" s="18"/>
+      <c r="AE73" s="18"/>
+      <c r="AF73" s="18"/>
+      <c r="AG73" s="18"/>
+      <c r="AH73" s="18"/>
+      <c r="AI73" s="18"/>
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+      <c r="AL73" s="18"/>
+      <c r="AM73" s="18"/>
+      <c r="AN73" s="18"/>
+      <c r="AO73" s="18"/>
+      <c r="AP73" s="18"/>
+      <c r="AQ73" s="18"/>
+    </row>
+    <row r="74" spans="1:52" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC74" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="AD73" s="20"/>
-      <c r="AE73" s="20"/>
-      <c r="AF73" s="20"/>
-    </row>
-    <row r="74" spans="1:52" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B74" s="8" t="s">
+      <c r="AD74" s="20"/>
+      <c r="AE74" s="20"/>
+      <c r="AF74" s="20"/>
+    </row>
+    <row r="75" spans="1:52" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8" t="s">
+      <c r="C75" s="8"/>
+      <c r="D75" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8" t="s">
+      <c r="E75" s="8"/>
+      <c r="F75" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8" t="s">
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8" t="s">
+      <c r="K75" s="8"/>
+      <c r="L75" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M74" s="8"/>
-      <c r="N74" s="8" t="s">
+      <c r="M75" s="8"/>
+      <c r="N75" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O74" s="8" t="s">
+      <c r="O75" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P74" s="8" t="s">
+      <c r="P75" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Q74" s="8" t="s">
+      <c r="Q75" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="R74" s="8" t="s">
+      <c r="R75" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="S74" s="8" t="s">
+      <c r="S75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="T74" s="9" t="s">
+      <c r="T75" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="U74" s="9" t="s">
+      <c r="U75" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="V74" s="8" t="s">
+      <c r="V75" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="W74" s="9" t="s">
+      <c r="W75" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="X74" s="9" t="s">
+      <c r="X75" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="Y74" s="8" t="s">
+      <c r="Y75" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Z74" s="8" t="s">
+      <c r="Z75" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AA74" s="8" t="s">
+      <c r="AA75" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AB74" s="8" t="s">
+      <c r="AB75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AC74" s="9" t="s">
+      <c r="AC75" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="AD74" s="9" t="s">
+      <c r="AD75" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="AE74" s="9" t="s">
+      <c r="AE75" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="AF74" s="9" t="s">
+      <c r="AF75" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="AG74" s="9" t="s">
+      <c r="AG75" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="AH74" s="9" t="s">
+      <c r="AH75" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="AI74" s="9" t="s">
+      <c r="AI75" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="AJ74" s="9" t="s">
+      <c r="AJ75" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="AK74" s="9" t="s">
+      <c r="AK75" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="AL74" s="9" t="s">
+      <c r="AL75" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="AM74" s="9" t="s">
+      <c r="AM75" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="AN74" s="9" t="s">
+      <c r="AN75" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="AO74" s="9" t="s">
+      <c r="AO75" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="AP74" s="9" t="s">
+      <c r="AP75" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="AQ74" s="9" t="s">
+      <c r="AQ75" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="AR74" s="9" t="s">
+      <c r="AR75" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="AS74" s="9" t="s">
+      <c r="AS75" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="AT74" s="9" t="s">
+      <c r="AT75" s="9" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C75" s="7">
-        <v>24</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I75" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J75" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K75" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="L75" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="M75" s="7">
-        <v>24</v>
-      </c>
-      <c r="N75" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="O75" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="P75" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q75" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="R75" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="S75" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="T75" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="U75" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="V75" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="W75" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="X75" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y75" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z75" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA75" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB75" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC75" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD75" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="AE75" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF75" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG75" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="AH75" s="24" t="s">
-        <v>335</v>
-      </c>
-      <c r="AI75" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="AJ75" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AK75" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL75" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AM75" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AN75" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AO75" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP75" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AR75" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="AS75" s="24" t="s">
-        <v>335</v>
-      </c>
-      <c r="AT75" s="7" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>226</v>
@@ -6291,7 +6280,7 @@
         <v>124</v>
       </c>
       <c r="O76" s="7" t="s">
-        <v>324</v>
+        <v>228</v>
       </c>
       <c r="P76" s="7" t="s">
         <v>133</v>
@@ -6306,10 +6295,10 @@
         <v>75</v>
       </c>
       <c r="T76" s="24" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="U76" s="7" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="V76" s="7" t="s">
         <v>130</v>
@@ -6333,22 +6322,22 @@
         <v>75</v>
       </c>
       <c r="AC76" s="7" t="s">
-        <v>325</v>
+        <v>230</v>
       </c>
       <c r="AD76" s="7" t="s">
-        <v>326</v>
+        <v>231</v>
       </c>
       <c r="AE76" s="7" t="s">
-        <v>263</v>
+        <v>183</v>
       </c>
       <c r="AF76" s="7" t="s">
         <v>141</v>
       </c>
       <c r="AG76" s="24" t="s">
-        <v>327</v>
+        <v>224</v>
       </c>
       <c r="AH76" s="24" t="s">
-        <v>291</v>
+        <v>335</v>
       </c>
       <c r="AI76" s="7" t="s">
         <v>218</v>
@@ -6375,18 +6364,18 @@
         <v>130</v>
       </c>
       <c r="AR76" s="7" t="s">
-        <v>328</v>
+        <v>233</v>
       </c>
       <c r="AS76" s="24" t="s">
-        <v>291</v>
+        <v>335</v>
       </c>
       <c r="AT76" s="7" t="s">
-        <v>329</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>236</v>
+        <v>268</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>226</v>
@@ -6425,7 +6414,7 @@
         <v>124</v>
       </c>
       <c r="O77" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="P77" s="7" t="s">
         <v>133</v>
@@ -6440,7 +6429,7 @@
         <v>75</v>
       </c>
       <c r="T77" s="24" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>34</v>
@@ -6467,10 +6456,10 @@
         <v>75</v>
       </c>
       <c r="AC77" s="7" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="AD77" s="7" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AE77" s="7" t="s">
         <v>263</v>
@@ -6479,10 +6468,10 @@
         <v>141</v>
       </c>
       <c r="AG77" s="24" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="AH77" s="24" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="AI77" s="7" t="s">
         <v>218</v>
@@ -6506,24 +6495,21 @@
         <v>135</v>
       </c>
       <c r="AP77" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ77" s="7" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="AR77" s="7" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="AS77" s="24" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="AT77" s="7" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="78" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>226</v>
@@ -6577,7 +6563,7 @@
         <v>75</v>
       </c>
       <c r="T78" s="24" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>34</v>
@@ -6604,10 +6590,10 @@
         <v>75</v>
       </c>
       <c r="AC78" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="AD78" s="7" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="AE78" s="7" t="s">
         <v>263</v>
@@ -6616,10 +6602,10 @@
         <v>141</v>
       </c>
       <c r="AG78" s="24" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="AH78" s="24" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="AI78" s="7" t="s">
         <v>218</v>
@@ -6649,18 +6635,18 @@
         <v>35</v>
       </c>
       <c r="AR78" s="7" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="AS78" s="24" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="AT78" s="7" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="79" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>226</v>
@@ -6714,7 +6700,7 @@
         <v>75</v>
       </c>
       <c r="T79" s="24" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="U79" s="7" t="s">
         <v>34</v>
@@ -6741,10 +6727,10 @@
         <v>75</v>
       </c>
       <c r="AC79" s="7" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="AD79" s="7" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="AE79" s="7" t="s">
         <v>263</v>
@@ -6753,10 +6739,10 @@
         <v>141</v>
       </c>
       <c r="AG79" s="24" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="AH79" s="24" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="AI79" s="7" t="s">
         <v>218</v>
@@ -6786,18 +6772,18 @@
         <v>35</v>
       </c>
       <c r="AR79" s="7" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="AS79" s="24" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="AT79" s="7" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="80" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>226</v>
@@ -6851,7 +6837,7 @@
         <v>75</v>
       </c>
       <c r="T80" s="24" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>34</v>
@@ -6878,22 +6864,22 @@
         <v>75</v>
       </c>
       <c r="AC80" s="7" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="AD80" s="7" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="AE80" s="7" t="s">
         <v>263</v>
       </c>
       <c r="AF80" s="7" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="AG80" s="24" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AH80" s="24" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AI80" s="7" t="s">
         <v>218</v>
@@ -6923,18 +6909,18 @@
         <v>35</v>
       </c>
       <c r="AR80" s="7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="AS80" s="24" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AT80" s="7" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>353</v>
+        <v>308</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>226</v>
@@ -6973,7 +6959,7 @@
         <v>124</v>
       </c>
       <c r="O81" s="7" t="s">
-        <v>361</v>
+        <v>330</v>
       </c>
       <c r="P81" s="7" t="s">
         <v>133</v>
@@ -6988,7 +6974,7 @@
         <v>75</v>
       </c>
       <c r="T81" s="24" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>34</v>
@@ -7000,7 +6986,7 @@
         <v>141</v>
       </c>
       <c r="X81" s="7" t="s">
-        <v>363</v>
+        <v>229</v>
       </c>
       <c r="Y81" s="7" t="s">
         <v>133</v>
@@ -7015,10 +7001,10 @@
         <v>75</v>
       </c>
       <c r="AC81" s="7" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="AD81" s="7" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="AE81" s="7" t="s">
         <v>263</v>
@@ -7027,10 +7013,10 @@
         <v>77</v>
       </c>
       <c r="AG81" s="24" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="AH81" s="24" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="AI81" s="7" t="s">
         <v>218</v>
@@ -7060,16 +7046,19 @@
         <v>35</v>
       </c>
       <c r="AR81" s="7" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="AS81" s="24" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="AT81" s="7" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="82" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>353</v>
+      </c>
       <c r="B82" s="7" t="s">
         <v>226</v>
       </c>
@@ -7083,7 +7072,7 @@
         <v>121</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>422</v>
+        <v>226</v>
       </c>
       <c r="G82" s="7" t="s">
         <v>121</v>
@@ -7107,7 +7096,7 @@
         <v>124</v>
       </c>
       <c r="O82" s="7" t="s">
-        <v>423</v>
+        <v>361</v>
       </c>
       <c r="P82" s="7" t="s">
         <v>133</v>
@@ -7122,7 +7111,7 @@
         <v>75</v>
       </c>
       <c r="T82" s="24" t="s">
-        <v>292</v>
+        <v>362</v>
       </c>
       <c r="U82" s="7" t="s">
         <v>34</v>
@@ -7134,7 +7123,7 @@
         <v>141</v>
       </c>
       <c r="X82" s="7" t="s">
-        <v>229</v>
+        <v>363</v>
       </c>
       <c r="Y82" s="7" t="s">
         <v>133</v>
@@ -7149,10 +7138,10 @@
         <v>75</v>
       </c>
       <c r="AC82" s="7" t="s">
-        <v>419</v>
+        <v>364</v>
       </c>
       <c r="AD82" s="7" t="s">
-        <v>420</v>
+        <v>365</v>
       </c>
       <c r="AE82" s="7" t="s">
         <v>263</v>
@@ -7160,11 +7149,11 @@
       <c r="AF82" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="AG82" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="AH82" s="7" t="s">
-        <v>335</v>
+      <c r="AG82" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="AH82" s="24" t="s">
+        <v>367</v>
       </c>
       <c r="AI82" s="7" t="s">
         <v>218</v>
@@ -7188,34 +7177,168 @@
         <v>135</v>
       </c>
       <c r="AP82" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ82" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR82" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="AS82" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT82" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="83" spans="1:46" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" s="7">
+        <v>24</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I83" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J83" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K83" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L83" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="M83" s="7">
+        <v>24</v>
+      </c>
+      <c r="N83" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="O83" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="P83" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q83" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="T83" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y83" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z83" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA83" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB83" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC83" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="AE83" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AF83" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG83" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH83" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="AI83" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="AJ83" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK83" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AL83" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AM83" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN83" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO83" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP83" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AS82" s="7" t="s">
+      <c r="AS83" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="AT82" s="7" t="s">
+      <c r="AT83" s="7" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="85" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="Y85" s="7"/>
-      <c r="Z85" s="7"/>
-      <c r="AA85" s="7"/>
-      <c r="AB85" s="7"/>
-      <c r="AC85" s="7"/>
-      <c r="AD85" s="7"/>
-      <c r="AE85" s="7"/>
-      <c r="AF85" s="7"/>
-      <c r="AG85" s="7"/>
-      <c r="AH85" s="7"/>
-      <c r="AI85" s="7"/>
-      <c r="AJ85" s="10"/>
-      <c r="AK85" s="10"/>
-      <c r="AL85" s="10"/>
-      <c r="AM85" s="10"/>
-      <c r="AN85" s="10"/>
-      <c r="AO85" s="10"/>
-      <c r="AP85" s="10"/>
+    <row r="86" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="7"/>
+      <c r="AC86" s="7"/>
+      <c r="AD86" s="7"/>
+      <c r="AE86" s="7"/>
+      <c r="AF86" s="7"/>
+      <c r="AG86" s="7"/>
+      <c r="AH86" s="7"/>
+      <c r="AI86" s="7"/>
+      <c r="AJ86" s="10"/>
+      <c r="AK86" s="10"/>
+      <c r="AL86" s="10"/>
+      <c r="AM86" s="10"/>
+      <c r="AN86" s="10"/>
+      <c r="AO86" s="10"/>
+      <c r="AP86" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>